<commit_message>
test modification excel depuis github desktop
</commit_message>
<xml_diff>
--- a/usage-statistics/accounts-annotations.xlsx
+++ b/usage-statistics/accounts-annotations.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tparment/git/r2lab-misc/usage-statistics/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="680" windowWidth="23460" windowHeight="27300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="accounts-annotations.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="202">
   <si>
     <t>id=001</t>
   </si>
@@ -630,6 +625,9 @@
   </si>
   <si>
     <t>Leba-</t>
+  </si>
+  <si>
+    <t>ignore</t>
   </si>
 </sst>
 </file>
@@ -727,14 +725,14 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1075,10 +1073,10 @@
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="1" customWidth="1"/>
@@ -1087,7 +1085,7 @@
     <col min="7" max="7" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>183</v>
       </c>
@@ -1122,7 +1120,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>2016</v>
       </c>
@@ -1153,8 +1151,11 @@
       <c r="J2" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K2" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>2016</v>
       </c>
@@ -1186,7 +1187,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>2016</v>
       </c>
@@ -1218,7 +1219,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>2016</v>
       </c>
@@ -1250,7 +1251,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>2016</v>
       </c>
@@ -1282,7 +1283,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>2016</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>2016</v>
       </c>
@@ -1346,7 +1347,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>2016</v>
       </c>
@@ -1378,7 +1379,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>2016</v>
       </c>
@@ -1410,7 +1411,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>2016</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>2016</v>
       </c>
@@ -1474,7 +1475,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>2016</v>
       </c>
@@ -1506,7 +1507,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>2016</v>
       </c>
@@ -1538,7 +1539,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>2016</v>
       </c>
@@ -1570,7 +1571,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>2016</v>
       </c>
@@ -1602,7 +1603,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" s="1">
         <v>2016</v>
       </c>
@@ -1634,7 +1635,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" s="1">
         <v>2017</v>
       </c>
@@ -1666,7 +1667,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" s="1">
         <v>2017</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" s="1">
         <v>2017</v>
       </c>
@@ -1730,7 +1731,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <v>2017</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" s="1">
         <v>2017</v>
       </c>
@@ -1794,7 +1795,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" s="1">
         <v>2017</v>
       </c>
@@ -1826,7 +1827,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" s="1">
         <v>2017</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" s="1">
         <v>2017</v>
       </c>
@@ -1890,7 +1891,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" s="1">
         <v>2017</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" s="1">
         <v>2017</v>
       </c>
@@ -1957,7 +1958,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" s="1">
         <v>2017</v>
       </c>
@@ -1989,7 +1990,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" s="1">
         <v>2017</v>
       </c>
@@ -2021,7 +2022,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" s="1">
         <v>2017</v>
       </c>
@@ -2053,7 +2054,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" s="1">
         <v>2017</v>
       </c>
@@ -2085,7 +2086,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" s="1">
         <v>2017</v>
       </c>
@@ -2117,7 +2118,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>2017</v>
       </c>
@@ -2149,7 +2150,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>2017</v>
       </c>
@@ -2181,7 +2182,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>2017</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>2017</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>2017</v>
       </c>
@@ -2277,7 +2278,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>2017</v>
       </c>
@@ -2309,7 +2310,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>2017</v>
       </c>
@@ -2341,7 +2342,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <v>2017</v>
       </c>
@@ -2373,7 +2374,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>2017</v>
       </c>
@@ -2405,7 +2406,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>2017</v>
       </c>
@@ -2437,7 +2438,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>2017</v>
       </c>
@@ -2469,7 +2470,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>2017</v>
       </c>
@@ -2501,7 +2502,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>2017</v>
       </c>
@@ -2533,7 +2534,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>2017</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>2017</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>2017</v>
       </c>
@@ -2629,7 +2630,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49" s="1">
         <v>2017</v>
       </c>
@@ -2661,7 +2662,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11">
       <c r="A50" s="1">
         <v>2017</v>
       </c>
@@ -2693,7 +2694,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11">
       <c r="A51" s="1">
         <v>2017</v>
       </c>
@@ -2725,7 +2726,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11">
       <c r="A52" s="1">
         <v>2017</v>
       </c>
@@ -2757,7 +2758,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11">
       <c r="A53" s="1">
         <v>2017</v>
       </c>
@@ -2789,7 +2790,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11">
       <c r="A54" s="1">
         <v>2017</v>
       </c>
@@ -2821,7 +2822,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11">
       <c r="A55" s="1">
         <v>2017</v>
       </c>
@@ -2856,7 +2857,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56" s="1">
         <v>2017</v>
       </c>
@@ -2888,7 +2889,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11">
       <c r="A57" s="1">
         <v>2017</v>
       </c>
@@ -2920,7 +2921,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11">
       <c r="A58" s="1">
         <v>2017</v>
       </c>
@@ -2952,7 +2953,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59" s="1">
         <v>2017</v>
       </c>
@@ -2984,7 +2985,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11">
       <c r="A60" s="1">
         <v>2017</v>
       </c>
@@ -3016,7 +3017,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11">
       <c r="A61" s="1">
         <v>2017</v>
       </c>
@@ -3048,7 +3049,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11">
       <c r="A62" s="1">
         <v>2017</v>
       </c>
@@ -3080,7 +3081,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11">
       <c r="A63" s="1">
         <v>2017</v>
       </c>
@@ -3112,7 +3113,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11">
       <c r="A64" s="1">
         <v>2017</v>
       </c>
@@ -3144,7 +3145,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>2017</v>
       </c>
@@ -3176,7 +3177,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>2017</v>
       </c>
@@ -3208,7 +3209,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>2017</v>
       </c>
@@ -3240,7 +3241,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>2017</v>
       </c>
@@ -3272,7 +3273,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>2017</v>
       </c>
@@ -3304,7 +3305,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>2017</v>
       </c>
@@ -3336,7 +3337,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>2017</v>
       </c>
@@ -3368,7 +3369,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>2017</v>
       </c>
@@ -3400,7 +3401,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>2017</v>
       </c>
@@ -3432,7 +3433,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>2017</v>
       </c>
@@ -3464,7 +3465,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>2017</v>
       </c>
@@ -3496,7 +3497,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>2018</v>
       </c>
@@ -3528,7 +3529,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>2018</v>
       </c>
@@ -3560,7 +3561,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>2018</v>
       </c>
@@ -3592,7 +3593,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>2018</v>
       </c>
@@ -3624,7 +3625,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>2018</v>
       </c>
@@ -3656,7 +3657,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>2018</v>
       </c>
@@ -3688,7 +3689,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>2018</v>
       </c>
@@ -3720,7 +3721,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>2018</v>
       </c>
@@ -3754,6 +3755,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
accounts-annotations has 86 new entries to be classified
</commit_message>
<xml_diff>
--- a/usage-statistics/accounts-annotations.xlsx
+++ b/usage-statistics/accounts-annotations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dabbous/git/r2lab-misc/usage-statistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tparment/git/r2lab-misc/usage-statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1CFF68-95E2-8B48-A9CD-3E33D1F5C1B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71944C0A-C16F-EE45-A3B1-B8BBC2587DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="500" windowWidth="29000" windowHeight="17060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accounts-annotations.csv" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="334">
   <si>
     <t>id=001</t>
   </si>
@@ -772,13 +772,271 @@
   </si>
   <si>
     <t>Netherlands</t>
+  </si>
+  <si>
+    <t>arouk.osama@gmail.com</t>
+  </si>
+  <si>
+    <t>raymond.knopp@eurecom.fr</t>
+  </si>
+  <si>
+    <t>ftester@wall2.ilabt.iminds.be.stub</t>
+  </si>
+  <si>
+    <t>wvdemeer@wall2.ilabt.iminds.be.stub</t>
+  </si>
+  <si>
+    <t>jskim14@mwnl.snu.ac.kr</t>
+  </si>
+  <si>
+    <t>vincent.verleun@kpn.com</t>
+  </si>
+  <si>
+    <t>mohammed.jabi.1@ens.etsmtl.ca</t>
+  </si>
+  <si>
+    <t>raphael.defosseux@openairinterface.org</t>
+  </si>
+  <si>
+    <t>gabriele.perrone@openairinterface.org</t>
+  </si>
+  <si>
+    <t>adeel-khalid.siddiqui@etu.univ-cotedazur.fr</t>
+  </si>
+  <si>
+    <t>sumit.kumar@uni.lu</t>
+  </si>
+  <si>
+    <t>avenka24@ncsu.edu</t>
+  </si>
+  <si>
+    <t>houssam.elbouanani@inria.fr</t>
+  </si>
+  <si>
+    <t>jaroslaw.frelek@gmail.com</t>
+  </si>
+  <si>
+    <t>jithsudha@gmail.com</t>
+  </si>
+  <si>
+    <t>rjanowski@poczta.wwsi.edu.pl</t>
+  </si>
+  <si>
+    <t>fmmsousa@ilabt.imec.be.stub</t>
+  </si>
+  <si>
+    <t>dhaval.patel@ahduni.edu.in</t>
+  </si>
+  <si>
+    <t>lfarizav@gmail.com</t>
+  </si>
+  <si>
+    <t>wborbaneto@gmail.com</t>
+  </si>
+  <si>
+    <t>canina.assya@gmail.com</t>
+  </si>
+  <si>
+    <t>wilson.borba-da-rocha-neto@inria.fr</t>
+  </si>
+  <si>
+    <t>weverton.medeiros@ee.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t>serban_rares@yahoo.com</t>
+  </si>
+  <si>
+    <t>matteo.vincenzi@upc.edu</t>
+  </si>
+  <si>
+    <t>mamoutou.diarra@inria.fr</t>
+  </si>
+  <si>
+    <t>anup.kiran@outlook.com</t>
+  </si>
+  <si>
+    <t>xavier13@vt.edu</t>
+  </si>
+  <si>
+    <t>karnap1996@gmail.com</t>
+  </si>
+  <si>
+    <t>avlahov66@gmail.com</t>
+  </si>
+  <si>
+    <t>remi.hardy@openairinterface.org</t>
+  </si>
+  <si>
+    <t>leigh.porter@roke.co.uk</t>
+  </si>
+  <si>
+    <t>jotero@idtolu.com</t>
+  </si>
+  <si>
+    <t>louis.barbe@eurecom.fr</t>
+  </si>
+  <si>
+    <t>fco96mtz@gmail.com</t>
+  </si>
+  <si>
+    <t>docente_investigador9@corposucre.edu.co</t>
+  </si>
+  <si>
+    <t>sucrelab5g@gmail.com</t>
+  </si>
+  <si>
+    <t>anechoicspoof@gmail.com</t>
+  </si>
+  <si>
+    <t>mirado.rabenasolo@telecom-paris.fr</t>
+  </si>
+  <si>
+    <t>javier.velasquezgil@gmail.com</t>
+  </si>
+  <si>
+    <t>paul.olivier@eurecom.fr</t>
+  </si>
+  <si>
+    <t>1826273875@qq.com</t>
+  </si>
+  <si>
+    <t>2625936438@qq.com</t>
+  </si>
+  <si>
+    <t>teo.hays@protonmail.com</t>
+  </si>
+  <si>
+    <t>songrittom@gmail.com</t>
+  </si>
+  <si>
+    <t>ahmad.bazzi@ceva-dsp.com</t>
+  </si>
+  <si>
+    <t>nahel12789@gmail.com</t>
+  </si>
+  <si>
+    <t>abedifarv@gmail.com</t>
+  </si>
+  <si>
+    <t>mhd.nouri@yahoo.com</t>
+  </si>
+  <si>
+    <t>huy.ngo@eurecom.fr</t>
+  </si>
+  <si>
+    <t>ramon.fontes@imd.ufrn.br</t>
+  </si>
+  <si>
+    <t>aqadeer000@citymail.cuny.edu</t>
+  </si>
+  <si>
+    <t>arthur.bureau1@etu.univ-nantes.fr</t>
+  </si>
+  <si>
+    <t>pascal.tempier@inria.fr</t>
+  </si>
+  <si>
+    <t>ftester@ilabt.imec.be.stub</t>
+  </si>
+  <si>
+    <t>mohamed.lahsini@inria.fr</t>
+  </si>
+  <si>
+    <t>raza.ul-mustafa@inria.fr</t>
+  </si>
+  <si>
+    <t>theodoros.tsourdinis@lip6.fr</t>
+  </si>
+  <si>
+    <t>vinod.khandkar@inria.fr</t>
+  </si>
+  <si>
+    <t>yhadjadj@irisa.fr</t>
+  </si>
+  <si>
+    <t>anne-josiane.kouam-djuigne@inria.fr</t>
+  </si>
+  <si>
+    <t>noschmid@student.ethz.ch</t>
+  </si>
+  <si>
+    <t>mamoutou.diarra@hivenet.com</t>
+  </si>
+  <si>
+    <t>robbie.drage@spsautomation.com</t>
+  </si>
+  <si>
+    <t>sindi@innovatechtelecom.com</t>
+  </si>
+  <si>
+    <t>boutiba@eurecom.fr</t>
+  </si>
+  <si>
+    <t>g.pantaleo5@studenti.poliba.it</t>
+  </si>
+  <si>
+    <t>markrosenbaum@wearehackerone.com</t>
+  </si>
+  <si>
+    <t>jose.moura@iscte-iul.pt</t>
+  </si>
+  <si>
+    <t>sagar.arora@eurecom.fr</t>
+  </si>
+  <si>
+    <t>aya.moheddine@inria.fr</t>
+  </si>
+  <si>
+    <t>jiali.xu@inria.fr</t>
+  </si>
+  <si>
+    <t>selma.yahia@inria.fr</t>
+  </si>
+  <si>
+    <t>amamiyassir@gmail.com</t>
+  </si>
+  <si>
+    <t>rakesh.mundlamuri@eurecom.fr</t>
+  </si>
+  <si>
+    <t>nmkirimi@gmail.com</t>
+  </si>
+  <si>
+    <t>sanaa.ghandi@inria.fr</t>
+  </si>
+  <si>
+    <t>gitlab.runner@turletti.com</t>
+  </si>
+  <si>
+    <t>nbhatia3@ucsc.edu</t>
+  </si>
+  <si>
+    <t>saadtzl.2002@gmail.com</t>
+  </si>
+  <si>
+    <t>parsa.rajabzadeh@nokia.com</t>
+  </si>
+  <si>
+    <t>gallenmu@net.in.tum.de</t>
+  </si>
+  <si>
+    <t>fitowh@gmail.com</t>
+  </si>
+  <si>
+    <t>mattia.ciaccia@inria.fr</t>
+  </si>
+  <si>
+    <t>maros.plsik@tuvsud.com</t>
+  </si>
+  <si>
+    <t>mohammadbagher.tavassoli-kejani@inria.fr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -823,6 +1081,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF839496"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -853,7 +1117,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -864,21 +1128,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1227,10 +1485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K136"/>
+  <dimension ref="A1:K220"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G106" sqref="G106"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="G212" sqref="G212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1238,7 +1496,7 @@
     <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" customWidth="1"/>
+    <col min="5" max="5" width="51.33203125" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="1"/>
     <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
     <col min="8" max="10" width="10.83203125" style="1"/>
@@ -1424,7 +1682,7 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -1456,7 +1714,7 @@
       <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1488,7 +1746,7 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1520,7 +1778,7 @@
       <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1552,7 +1810,7 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1584,7 +1842,7 @@
       <c r="E11" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1616,7 +1874,7 @@
       <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1648,7 +1906,7 @@
       <c r="E13" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>139</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1680,7 +1938,7 @@
       <c r="E14" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1712,7 +1970,7 @@
       <c r="E15" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1744,7 +2002,7 @@
       <c r="E16" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1776,7 +2034,7 @@
       <c r="E17" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -1808,7 +2066,7 @@
       <c r="E18" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -1840,7 +2098,7 @@
       <c r="E19" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -1872,7 +2130,7 @@
       <c r="E20" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -1904,7 +2162,7 @@
       <c r="E21" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -1936,7 +2194,7 @@
       <c r="E22" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -1965,16 +2223,16 @@
       <c r="D23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H23" s="8" t="s">
+      <c r="G23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>162</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -1997,16 +2255,16 @@
       <c r="D24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H24" s="8" t="s">
+      <c r="F24" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>161</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -2029,16 +2287,16 @@
       <c r="D25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H25" s="8" t="s">
+      <c r="F25" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>161</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -2061,16 +2319,16 @@
       <c r="D26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G26" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H26" s="8" t="s">
+      <c r="G26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>162</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -2094,16 +2352,16 @@
       <c r="D27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H27" s="8" t="s">
+      <c r="F27" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>161</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -2126,16 +2384,16 @@
       <c r="D28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" t="s">
         <v>53</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H28" s="8" t="s">
+      <c r="F28" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>161</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -2158,16 +2416,16 @@
       <c r="D29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G29" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H29" s="8" t="s">
+      <c r="G29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>162</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -2190,16 +2448,16 @@
       <c r="D30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" t="s">
         <v>57</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G30" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H30" s="8" t="s">
+      <c r="G30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>162</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -2222,16 +2480,16 @@
       <c r="D31" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H31" s="8" t="s">
+      <c r="F31" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>162</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2257,7 +2515,7 @@
       <c r="E32" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>141</v>
       </c>
       <c r="G32" s="1" t="s">
@@ -2289,7 +2547,7 @@
       <c r="E33" t="s">
         <v>63</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G33" s="1" t="s">
@@ -2321,7 +2579,7 @@
       <c r="E34" t="s">
         <v>65</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G34" s="1" t="s">
@@ -2353,7 +2611,7 @@
       <c r="E35" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G35" s="1" t="s">
@@ -2385,7 +2643,7 @@
       <c r="E36" t="s">
         <v>69</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G36" s="1" t="s">
@@ -2417,7 +2675,7 @@
       <c r="E37" t="s">
         <v>71</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="4" t="s">
         <v>142</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -2449,7 +2707,7 @@
       <c r="E38" t="s">
         <v>73</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G38" s="1" t="s">
@@ -2481,7 +2739,7 @@
       <c r="E39" t="s">
         <v>75</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="4" t="s">
         <v>141</v>
       </c>
       <c r="G39" s="1" t="s">
@@ -2513,7 +2771,7 @@
       <c r="E40" t="s">
         <v>77</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="4" t="s">
         <v>141</v>
       </c>
       <c r="G40" s="1" t="s">
@@ -2545,7 +2803,7 @@
       <c r="E41" t="s">
         <v>79</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="4" t="s">
         <v>143</v>
       </c>
       <c r="G41" s="1" t="s">
@@ -2577,7 +2835,7 @@
       <c r="E42" t="s">
         <v>81</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G42" s="1" t="s">
@@ -2609,7 +2867,7 @@
       <c r="E43" t="s">
         <v>83</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G43" s="1" t="s">
@@ -2641,10 +2899,10 @@
       <c r="E44" t="s">
         <v>85</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="G44" s="1" t="s">
         <v>159</v>
       </c>
       <c r="H44" s="1" t="s">
@@ -2673,7 +2931,7 @@
       <c r="E45" t="s">
         <v>87</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G45" s="1" t="s">
@@ -2705,7 +2963,7 @@
       <c r="E46" t="s">
         <v>89</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G46" s="1" t="s">
@@ -2737,10 +2995,10 @@
       <c r="E47" t="s">
         <v>91</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G47" s="1" t="s">
         <v>159</v>
       </c>
       <c r="H47" s="1" t="s">
@@ -2770,7 +3028,7 @@
       <c r="E48" t="s">
         <v>93</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="4" t="s">
         <v>148</v>
       </c>
       <c r="G48" s="1" t="s">
@@ -2802,7 +3060,7 @@
       <c r="E49" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G49" s="1" t="s">
@@ -2834,7 +3092,7 @@
       <c r="E50" t="s">
         <v>97</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F50" s="4" t="s">
         <v>137</v>
       </c>
       <c r="G50" s="1" t="s">
@@ -5126,7 +5384,7 @@
       <c r="D122" s="1">
         <v>156</v>
       </c>
-      <c r="E122" s="6" t="s">
+      <c r="E122" s="5" t="s">
         <v>223</v>
       </c>
       <c r="F122" s="1" t="s">
@@ -5161,7 +5419,7 @@
       <c r="D123" s="1">
         <v>157</v>
       </c>
-      <c r="E123" s="6" t="s">
+      <c r="E123" s="5" t="s">
         <v>224</v>
       </c>
       <c r="F123" s="1" t="s">
@@ -5179,7 +5437,7 @@
       <c r="J123" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="K123" s="9" t="s">
+      <c r="K123" s="6" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5196,7 +5454,7 @@
       <c r="D124" s="1">
         <v>158</v>
       </c>
-      <c r="E124" s="6" t="s">
+      <c r="E124" s="5" t="s">
         <v>225</v>
       </c>
       <c r="F124" s="1" t="s">
@@ -5231,7 +5489,7 @@
       <c r="D125" s="1">
         <v>159</v>
       </c>
-      <c r="E125" s="6" t="s">
+      <c r="E125" s="5" t="s">
         <v>226</v>
       </c>
       <c r="F125" s="1" t="s">
@@ -5263,7 +5521,7 @@
       <c r="D126" s="1">
         <v>160</v>
       </c>
-      <c r="E126" s="6" t="s">
+      <c r="E126" s="5" t="s">
         <v>227</v>
       </c>
       <c r="F126" s="1" t="s">
@@ -5351,7 +5609,7 @@
       <c r="J128" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="K128" s="9" t="s">
+      <c r="K128" s="6" t="s">
         <v>242</v>
       </c>
     </row>
@@ -5418,7 +5676,7 @@
       <c r="J130" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="K130" s="10" t="s">
+      <c r="K130" s="7" t="s">
         <v>243</v>
       </c>
     </row>
@@ -5485,7 +5743,7 @@
       <c r="J132" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="K132" s="9" t="s">
+      <c r="K132" s="6" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5502,7 +5760,7 @@
       <c r="D133" s="1">
         <v>167</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E133" s="5" t="s">
         <v>234</v>
       </c>
       <c r="F133" s="1" t="s">
@@ -5537,7 +5795,7 @@
       <c r="D134" s="1">
         <v>168</v>
       </c>
-      <c r="E134" s="6" t="s">
+      <c r="E134" s="5" t="s">
         <v>246</v>
       </c>
       <c r="F134" s="1" t="s">
@@ -5556,8 +5814,1209 @@
         <v>161</v>
       </c>
     </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A135" s="8">
+        <v>2017</v>
+      </c>
+      <c r="B135" s="8">
+        <v>4</v>
+      </c>
+      <c r="C135" s="8">
+        <v>11</v>
+      </c>
+      <c r="E135" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E136" s="6"/>
+      <c r="A136" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B136" s="8">
+        <v>4</v>
+      </c>
+      <c r="C136" s="8">
+        <v>10</v>
+      </c>
+      <c r="E136" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B137" s="8">
+        <v>4</v>
+      </c>
+      <c r="C137" s="8">
+        <v>18</v>
+      </c>
+      <c r="E137" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B138" s="8">
+        <v>4</v>
+      </c>
+      <c r="C138" s="8">
+        <v>19</v>
+      </c>
+      <c r="E138" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B139" s="8">
+        <v>4</v>
+      </c>
+      <c r="C139" s="8">
+        <v>22</v>
+      </c>
+      <c r="E139" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A140" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B140" s="8">
+        <v>5</v>
+      </c>
+      <c r="C140" s="8">
+        <v>2</v>
+      </c>
+      <c r="E140" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B141" s="8">
+        <v>5</v>
+      </c>
+      <c r="C141" s="8">
+        <v>21</v>
+      </c>
+      <c r="E141" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A142" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B142" s="8">
+        <v>7</v>
+      </c>
+      <c r="C142" s="8">
+        <v>9</v>
+      </c>
+      <c r="E142" s="8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B143" s="8">
+        <v>10</v>
+      </c>
+      <c r="C143" s="8">
+        <v>7</v>
+      </c>
+      <c r="E143" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B144" s="8">
+        <v>10</v>
+      </c>
+      <c r="C144" s="8">
+        <v>24</v>
+      </c>
+      <c r="E144" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B145" s="8">
+        <v>11</v>
+      </c>
+      <c r="C145" s="8">
+        <v>5</v>
+      </c>
+      <c r="E145" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B146" s="8">
+        <v>11</v>
+      </c>
+      <c r="C146" s="8">
+        <v>14</v>
+      </c>
+      <c r="E146" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B147" s="8">
+        <v>12</v>
+      </c>
+      <c r="C147" s="8">
+        <v>13</v>
+      </c>
+      <c r="E147" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B148" s="8">
+        <v>12</v>
+      </c>
+      <c r="C148" s="8">
+        <v>15</v>
+      </c>
+      <c r="E148" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B149" s="8">
+        <v>1</v>
+      </c>
+      <c r="C149" s="8">
+        <v>13</v>
+      </c>
+      <c r="E149" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B150" s="8">
+        <v>2</v>
+      </c>
+      <c r="C150" s="8">
+        <v>5</v>
+      </c>
+      <c r="E150" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B151" s="8">
+        <v>2</v>
+      </c>
+      <c r="C151" s="8">
+        <v>18</v>
+      </c>
+      <c r="E151" s="8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B152" s="8">
+        <v>2</v>
+      </c>
+      <c r="C152" s="8">
+        <v>22</v>
+      </c>
+      <c r="E152" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B153" s="8">
+        <v>2</v>
+      </c>
+      <c r="C153" s="8">
+        <v>25</v>
+      </c>
+      <c r="E153" s="8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B154" s="8">
+        <v>2</v>
+      </c>
+      <c r="C154" s="8">
+        <v>27</v>
+      </c>
+      <c r="E154" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B155" s="8">
+        <v>2</v>
+      </c>
+      <c r="C155" s="8">
+        <v>28</v>
+      </c>
+      <c r="E155" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B156" s="8">
+        <v>3</v>
+      </c>
+      <c r="C156" s="8">
+        <v>2</v>
+      </c>
+      <c r="E156" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B157" s="8">
+        <v>3</v>
+      </c>
+      <c r="C157" s="8">
+        <v>4</v>
+      </c>
+      <c r="E157" s="8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B158" s="8">
+        <v>3</v>
+      </c>
+      <c r="C158" s="8">
+        <v>5</v>
+      </c>
+      <c r="E158" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B159" s="8">
+        <v>3</v>
+      </c>
+      <c r="C159" s="8">
+        <v>20</v>
+      </c>
+      <c r="E159" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B160" s="8">
+        <v>3</v>
+      </c>
+      <c r="C160" s="8">
+        <v>20</v>
+      </c>
+      <c r="E160" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B161" s="8">
+        <v>4</v>
+      </c>
+      <c r="C161" s="8">
+        <v>2</v>
+      </c>
+      <c r="E161" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B162" s="8">
+        <v>5</v>
+      </c>
+      <c r="C162" s="8">
+        <v>8</v>
+      </c>
+      <c r="E162" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B163" s="8">
+        <v>6</v>
+      </c>
+      <c r="C163" s="8">
+        <v>2</v>
+      </c>
+      <c r="E163" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B164" s="8">
+        <v>6</v>
+      </c>
+      <c r="C164" s="8">
+        <v>3</v>
+      </c>
+      <c r="E164" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B165" s="8">
+        <v>6</v>
+      </c>
+      <c r="C165" s="8">
+        <v>10</v>
+      </c>
+      <c r="E165" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B166" s="8">
+        <v>7</v>
+      </c>
+      <c r="C166" s="8">
+        <v>2</v>
+      </c>
+      <c r="E166" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B167" s="8">
+        <v>8</v>
+      </c>
+      <c r="C167" s="8">
+        <v>31</v>
+      </c>
+      <c r="E167" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B168" s="8">
+        <v>11</v>
+      </c>
+      <c r="C168" s="8">
+        <v>16</v>
+      </c>
+      <c r="E168" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B169" s="8">
+        <v>11</v>
+      </c>
+      <c r="C169" s="8">
+        <v>23</v>
+      </c>
+      <c r="E169" s="8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B170" s="8">
+        <v>11</v>
+      </c>
+      <c r="C170" s="8">
+        <v>27</v>
+      </c>
+      <c r="E170" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B171" s="8">
+        <v>11</v>
+      </c>
+      <c r="C171" s="8">
+        <v>27</v>
+      </c>
+      <c r="E171" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B172" s="8">
+        <v>11</v>
+      </c>
+      <c r="C172" s="8">
+        <v>29</v>
+      </c>
+      <c r="E172" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B173" s="8">
+        <v>11</v>
+      </c>
+      <c r="C173" s="8">
+        <v>29</v>
+      </c>
+      <c r="E173" s="8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B174" s="8">
+        <v>1</v>
+      </c>
+      <c r="C174" s="8">
+        <v>20</v>
+      </c>
+      <c r="E174" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B175" s="8">
+        <v>3</v>
+      </c>
+      <c r="C175" s="8">
+        <v>31</v>
+      </c>
+      <c r="E175" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B176" s="8">
+        <v>4</v>
+      </c>
+      <c r="C176" s="8">
+        <v>12</v>
+      </c>
+      <c r="E176" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B177" s="8">
+        <v>4</v>
+      </c>
+      <c r="C177" s="8">
+        <v>12</v>
+      </c>
+      <c r="E177" s="8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B178" s="8">
+        <v>5</v>
+      </c>
+      <c r="C178" s="8">
+        <v>4</v>
+      </c>
+      <c r="E178" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B179" s="8">
+        <v>5</v>
+      </c>
+      <c r="C179" s="8">
+        <v>6</v>
+      </c>
+      <c r="E179" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B180" s="8">
+        <v>5</v>
+      </c>
+      <c r="C180" s="8">
+        <v>25</v>
+      </c>
+      <c r="E180" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B181" s="8">
+        <v>5</v>
+      </c>
+      <c r="C181" s="8">
+        <v>26</v>
+      </c>
+      <c r="E181" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B182" s="8">
+        <v>6</v>
+      </c>
+      <c r="C182" s="8">
+        <v>6</v>
+      </c>
+      <c r="E182" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B183" s="8">
+        <v>6</v>
+      </c>
+      <c r="C183" s="8">
+        <v>19</v>
+      </c>
+      <c r="E183" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B184" s="8">
+        <v>7</v>
+      </c>
+      <c r="C184" s="8">
+        <v>15</v>
+      </c>
+      <c r="E184" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B185" s="8">
+        <v>9</v>
+      </c>
+      <c r="C185" s="8">
+        <v>15</v>
+      </c>
+      <c r="E185" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B186" s="8">
+        <v>10</v>
+      </c>
+      <c r="C186" s="8">
+        <v>19</v>
+      </c>
+      <c r="E186" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B187" s="8">
+        <v>11</v>
+      </c>
+      <c r="C187" s="8">
+        <v>22</v>
+      </c>
+      <c r="E187" s="8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B188" s="8">
+        <v>11</v>
+      </c>
+      <c r="C188" s="8">
+        <v>24</v>
+      </c>
+      <c r="E188" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B189" s="8">
+        <v>12</v>
+      </c>
+      <c r="C189" s="8">
+        <v>3</v>
+      </c>
+      <c r="E189" s="8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B190" s="8">
+        <v>3</v>
+      </c>
+      <c r="C190" s="8">
+        <v>23</v>
+      </c>
+      <c r="E190" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B191" s="8">
+        <v>6</v>
+      </c>
+      <c r="C191" s="8">
+        <v>29</v>
+      </c>
+      <c r="E191" s="8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B192" s="8">
+        <v>7</v>
+      </c>
+      <c r="C192" s="8">
+        <v>11</v>
+      </c>
+      <c r="E192" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B193" s="8">
+        <v>7</v>
+      </c>
+      <c r="C193" s="8">
+        <v>21</v>
+      </c>
+      <c r="E193" s="8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B194" s="8">
+        <v>9</v>
+      </c>
+      <c r="C194" s="8">
+        <v>13</v>
+      </c>
+      <c r="E194" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B195" s="8">
+        <v>9</v>
+      </c>
+      <c r="C195" s="8">
+        <v>16</v>
+      </c>
+      <c r="E195" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B196" s="8">
+        <v>9</v>
+      </c>
+      <c r="C196" s="8">
+        <v>29</v>
+      </c>
+      <c r="E196" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B197" s="8">
+        <v>12</v>
+      </c>
+      <c r="C197" s="8">
+        <v>12</v>
+      </c>
+      <c r="E197" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B198" s="8">
+        <v>12</v>
+      </c>
+      <c r="C198" s="8">
+        <v>13</v>
+      </c>
+      <c r="E198" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B199" s="8">
+        <v>12</v>
+      </c>
+      <c r="C199" s="8">
+        <v>20</v>
+      </c>
+      <c r="E199" s="8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B200" s="8">
+        <v>1</v>
+      </c>
+      <c r="C200" s="8">
+        <v>11</v>
+      </c>
+      <c r="E200" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B201" s="8">
+        <v>1</v>
+      </c>
+      <c r="C201" s="8">
+        <v>11</v>
+      </c>
+      <c r="E201" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B202" s="8">
+        <v>2</v>
+      </c>
+      <c r="C202" s="8">
+        <v>4</v>
+      </c>
+      <c r="E202" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B203" s="8">
+        <v>3</v>
+      </c>
+      <c r="C203" s="8">
+        <v>31</v>
+      </c>
+      <c r="E203" s="8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B204" s="8">
+        <v>4</v>
+      </c>
+      <c r="C204" s="8">
+        <v>28</v>
+      </c>
+      <c r="E204" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B205" s="8">
+        <v>9</v>
+      </c>
+      <c r="C205" s="8">
+        <v>12</v>
+      </c>
+      <c r="E205" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B206" s="8">
+        <v>9</v>
+      </c>
+      <c r="C206" s="8">
+        <v>12</v>
+      </c>
+      <c r="E206" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B207" s="8">
+        <v>10</v>
+      </c>
+      <c r="C207" s="8">
+        <v>11</v>
+      </c>
+      <c r="E207" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B208" s="8">
+        <v>10</v>
+      </c>
+      <c r="C208" s="8">
+        <v>25</v>
+      </c>
+      <c r="E208" s="8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B209" s="8">
+        <v>10</v>
+      </c>
+      <c r="C209" s="8">
+        <v>26</v>
+      </c>
+      <c r="E209" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B210" s="8">
+        <v>11</v>
+      </c>
+      <c r="C210" s="8">
+        <v>21</v>
+      </c>
+      <c r="E210" s="8" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B211" s="8">
+        <v>1</v>
+      </c>
+      <c r="C211" s="8">
+        <v>8</v>
+      </c>
+      <c r="E211" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B212" s="8">
+        <v>2</v>
+      </c>
+      <c r="C212" s="8">
+        <v>2</v>
+      </c>
+      <c r="E212" s="8" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B213" s="8">
+        <v>2</v>
+      </c>
+      <c r="C213" s="8">
+        <v>8</v>
+      </c>
+      <c r="E213" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B214" s="8">
+        <v>3</v>
+      </c>
+      <c r="C214" s="8">
+        <v>15</v>
+      </c>
+      <c r="E214" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B215" s="8">
+        <v>3</v>
+      </c>
+      <c r="C215" s="8">
+        <v>29</v>
+      </c>
+      <c r="E215" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B216" s="8">
+        <v>4</v>
+      </c>
+      <c r="C216" s="8">
+        <v>24</v>
+      </c>
+      <c r="E216" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B217" s="8">
+        <v>5</v>
+      </c>
+      <c r="C217" s="8">
+        <v>14</v>
+      </c>
+      <c r="E217" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B218" s="8">
+        <v>5</v>
+      </c>
+      <c r="C218" s="8">
+        <v>15</v>
+      </c>
+      <c r="E218" s="8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B219" s="8">
+        <v>5</v>
+      </c>
+      <c r="C219" s="8">
+        <v>22</v>
+      </c>
+      <c r="E219" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B220" s="8">
+        <v>6</v>
+      </c>
+      <c r="C220" s="8">
+        <v>20</v>
+      </c>
+      <c r="E220" s="8" t="s">
+        <v>333</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5567,6 +7026,7 @@
     <hyperlink ref="E125" r:id="rId4" xr:uid="{E11FAB11-FA2B-1F43-BBD9-DCF008AC5CD1}"/>
     <hyperlink ref="E126" r:id="rId5" xr:uid="{3EB2F7EB-F790-664D-B837-D3E3FB0757B6}"/>
     <hyperlink ref="E134" r:id="rId6" xr:uid="{1BD56906-84F7-3B49-84AA-A11760B0D79E}"/>
+    <hyperlink ref="E133" r:id="rId7" xr:uid="{8B4200FD-E008-6A49-9EBC-A49BF9ED620B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
more complete stats for 2021 → aug 2024
</commit_message>
<xml_diff>
--- a/usage-statistics/accounts-annotations.xlsx
+++ b/usage-statistics/accounts-annotations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tparment/git/r2lab-misc/usage-statistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dabbous/Documents/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71944C0A-C16F-EE45-A3B1-B8BBC2587DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CCE9C8-CA5C-1A4B-A361-F97AFE32A379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="500" windowWidth="29000" windowHeight="17060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="780" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accounts-annotations.csv" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="386">
   <si>
     <t>id=001</t>
   </si>
@@ -774,269 +774,425 @@
     <t>Netherlands</t>
   </si>
   <si>
+    <t>raymond.knopp@eurecom.fr</t>
+  </si>
+  <si>
+    <t>ftester@wall2.ilabt.iminds.be.stub</t>
+  </si>
+  <si>
+    <t>wvdemeer@wall2.ilabt.iminds.be.stub</t>
+  </si>
+  <si>
+    <t>jskim14@mwnl.snu.ac.kr</t>
+  </si>
+  <si>
+    <t>vincent.verleun@kpn.com</t>
+  </si>
+  <si>
+    <t>mohammed.jabi.1@ens.etsmtl.ca</t>
+  </si>
+  <si>
+    <t>raphael.defosseux@openairinterface.org</t>
+  </si>
+  <si>
+    <t>gabriele.perrone@openairinterface.org</t>
+  </si>
+  <si>
+    <t>adeel-khalid.siddiqui@etu.univ-cotedazur.fr</t>
+  </si>
+  <si>
+    <t>sumit.kumar@uni.lu</t>
+  </si>
+  <si>
+    <t>avenka24@ncsu.edu</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>houssam.elbouanani@inria.fr</t>
+  </si>
+  <si>
+    <t>jaroslaw.frelek@gmail.com</t>
+  </si>
+  <si>
+    <t>jithsudha@gmail.com</t>
+  </si>
+  <si>
+    <t>rjanowski@poczta.wwsi.edu.pl</t>
+  </si>
+  <si>
+    <t>fmmsousa@ilabt.imec.be.stub</t>
+  </si>
+  <si>
+    <t>dhaval.patel@ahduni.edu.in</t>
+  </si>
+  <si>
+    <t>lfarizav@gmail.com</t>
+  </si>
+  <si>
+    <t>wborbaneto@gmail.com</t>
+  </si>
+  <si>
+    <t>canina.assya@gmail.com</t>
+  </si>
+  <si>
+    <t>wilson.borba-da-rocha-neto@inria.fr</t>
+  </si>
+  <si>
+    <t>weverton.medeiros@ee.ufcg.edu.br</t>
+  </si>
+  <si>
+    <t>serban_rares@yahoo.com</t>
+  </si>
+  <si>
+    <t>matteo.vincenzi@upc.edu</t>
+  </si>
+  <si>
+    <t>mamoutou.diarra@inria.fr</t>
+  </si>
+  <si>
+    <t>anup.kiran@outlook.com</t>
+  </si>
+  <si>
+    <t>xavier13@vt.edu</t>
+  </si>
+  <si>
+    <t>karnap1996@gmail.com</t>
+  </si>
+  <si>
+    <t>avlahov66@gmail.com</t>
+  </si>
+  <si>
+    <t>remi.hardy@openairinterface.org</t>
+  </si>
+  <si>
+    <t>leigh.porter@roke.co.uk</t>
+  </si>
+  <si>
+    <t>jotero@idtolu.com</t>
+  </si>
+  <si>
+    <t>louis.barbe@eurecom.fr</t>
+  </si>
+  <si>
+    <t>fco96mtz@gmail.com</t>
+  </si>
+  <si>
+    <t>docente_investigador9@corposucre.edu.co</t>
+  </si>
+  <si>
+    <t>sucrelab5g@gmail.com</t>
+  </si>
+  <si>
+    <t>anechoicspoof@gmail.com</t>
+  </si>
+  <si>
+    <t>mirado.rabenasolo@telecom-paris.fr</t>
+  </si>
+  <si>
+    <t>javier.velasquezgil@gmail.com</t>
+  </si>
+  <si>
+    <t>paul.olivier@eurecom.fr</t>
+  </si>
+  <si>
+    <t>1826273875@qq.com</t>
+  </si>
+  <si>
+    <t>2625936438@qq.com</t>
+  </si>
+  <si>
+    <t>teo.hays@protonmail.com</t>
+  </si>
+  <si>
+    <t>songrittom@gmail.com</t>
+  </si>
+  <si>
+    <t>ahmad.bazzi@ceva-dsp.com</t>
+  </si>
+  <si>
+    <t>nahel12789@gmail.com</t>
+  </si>
+  <si>
+    <t>abedifarv@gmail.com</t>
+  </si>
+  <si>
+    <t>mhd.nouri@yahoo.com</t>
+  </si>
+  <si>
+    <t>huy.ngo@eurecom.fr</t>
+  </si>
+  <si>
+    <t>ramon.fontes@imd.ufrn.br</t>
+  </si>
+  <si>
+    <t>aqadeer000@citymail.cuny.edu</t>
+  </si>
+  <si>
+    <t>arthur.bureau1@etu.univ-nantes.fr</t>
+  </si>
+  <si>
+    <t>pascal.tempier@inria.fr</t>
+  </si>
+  <si>
+    <t>ftester@ilabt.imec.be.stub</t>
+  </si>
+  <si>
+    <t>mohamed.lahsini@inria.fr</t>
+  </si>
+  <si>
+    <t>raza.ul-mustafa@inria.fr</t>
+  </si>
+  <si>
+    <t>theodoros.tsourdinis@lip6.fr</t>
+  </si>
+  <si>
+    <t>vinod.khandkar@inria.fr</t>
+  </si>
+  <si>
+    <t>yhadjadj@irisa.fr</t>
+  </si>
+  <si>
+    <t>anne-josiane.kouam-djuigne@inria.fr</t>
+  </si>
+  <si>
+    <t>noschmid@student.ethz.ch</t>
+  </si>
+  <si>
+    <t>mamoutou.diarra@hivenet.com</t>
+  </si>
+  <si>
+    <t>robbie.drage@spsautomation.com</t>
+  </si>
+  <si>
+    <t>sindi@innovatechtelecom.com</t>
+  </si>
+  <si>
+    <t>boutiba@eurecom.fr</t>
+  </si>
+  <si>
+    <t>g.pantaleo5@studenti.poliba.it</t>
+  </si>
+  <si>
+    <t>markrosenbaum@wearehackerone.com</t>
+  </si>
+  <si>
+    <t>jose.moura@iscte-iul.pt</t>
+  </si>
+  <si>
+    <t>sagar.arora@eurecom.fr</t>
+  </si>
+  <si>
+    <t>aya.moheddine@inria.fr</t>
+  </si>
+  <si>
+    <t>jiali.xu@inria.fr</t>
+  </si>
+  <si>
+    <t>selma.yahia@inria.fr</t>
+  </si>
+  <si>
+    <t>amamiyassir@gmail.com</t>
+  </si>
+  <si>
+    <t>rakesh.mundlamuri@eurecom.fr</t>
+  </si>
+  <si>
+    <t>nmkirimi@gmail.com</t>
+  </si>
+  <si>
+    <t>sanaa.ghandi@inria.fr</t>
+  </si>
+  <si>
+    <t>gitlab.runner@turletti.com</t>
+  </si>
+  <si>
+    <t>nbhatia3@ucsc.edu</t>
+  </si>
+  <si>
+    <t>saadtzl.2002@gmail.com</t>
+  </si>
+  <si>
+    <t>parsa.rajabzadeh@nokia.com</t>
+  </si>
+  <si>
+    <t>gallenmu@net.in.tum.de</t>
+  </si>
+  <si>
+    <t>fitowh@gmail.com</t>
+  </si>
+  <si>
+    <t>mattia.ciaccia@inria.fr</t>
+  </si>
+  <si>
+    <t>maros.plsik@tuvsud.com</t>
+  </si>
+  <si>
+    <t>mohammadbagher.tavassoli-kejani@inria.fr</t>
+  </si>
+  <si>
     <t>arouk.osama@gmail.com</t>
   </si>
   <si>
-    <t>raymond.knopp@eurecom.fr</t>
-  </si>
-  <si>
-    <t>ftester@wall2.ilabt.iminds.be.stub</t>
-  </si>
-  <si>
-    <t>wvdemeer@wall2.ilabt.iminds.be.stub</t>
-  </si>
-  <si>
-    <t>jskim14@mwnl.snu.ac.kr</t>
-  </si>
-  <si>
-    <t>vincent.verleun@kpn.com</t>
-  </si>
-  <si>
-    <t>mohammed.jabi.1@ens.etsmtl.ca</t>
-  </si>
-  <si>
-    <t>raphael.defosseux@openairinterface.org</t>
-  </si>
-  <si>
-    <t>gabriele.perrone@openairinterface.org</t>
-  </si>
-  <si>
-    <t>adeel-khalid.siddiqui@etu.univ-cotedazur.fr</t>
-  </si>
-  <si>
-    <t>sumit.kumar@uni.lu</t>
-  </si>
-  <si>
-    <t>avenka24@ncsu.edu</t>
-  </si>
-  <si>
-    <t>houssam.elbouanani@inria.fr</t>
-  </si>
-  <si>
-    <t>jaroslaw.frelek@gmail.com</t>
-  </si>
-  <si>
-    <t>jithsudha@gmail.com</t>
-  </si>
-  <si>
-    <t>rjanowski@poczta.wwsi.edu.pl</t>
-  </si>
-  <si>
-    <t>fmmsousa@ilabt.imec.be.stub</t>
-  </si>
-  <si>
-    <t>dhaval.patel@ahduni.edu.in</t>
-  </si>
-  <si>
-    <t>lfarizav@gmail.com</t>
-  </si>
-  <si>
-    <t>wborbaneto@gmail.com</t>
-  </si>
-  <si>
-    <t>canina.assya@gmail.com</t>
-  </si>
-  <si>
-    <t>wilson.borba-da-rocha-neto@inria.fr</t>
-  </si>
-  <si>
-    <t>weverton.medeiros@ee.ufcg.edu.br</t>
-  </si>
-  <si>
-    <t>serban_rares@yahoo.com</t>
-  </si>
-  <si>
-    <t>matteo.vincenzi@upc.edu</t>
-  </si>
-  <si>
-    <t>mamoutou.diarra@inria.fr</t>
-  </si>
-  <si>
-    <t>anup.kiran@outlook.com</t>
-  </si>
-  <si>
-    <t>xavier13@vt.edu</t>
-  </si>
-  <si>
-    <t>karnap1996@gmail.com</t>
-  </si>
-  <si>
-    <t>avlahov66@gmail.com</t>
-  </si>
-  <si>
-    <t>remi.hardy@openairinterface.org</t>
-  </si>
-  <si>
-    <t>leigh.porter@roke.co.uk</t>
-  </si>
-  <si>
-    <t>jotero@idtolu.com</t>
-  </si>
-  <si>
-    <t>louis.barbe@eurecom.fr</t>
-  </si>
-  <si>
-    <t>fco96mtz@gmail.com</t>
-  </si>
-  <si>
-    <t>docente_investigador9@corposucre.edu.co</t>
-  </si>
-  <si>
-    <t>sucrelab5g@gmail.com</t>
-  </si>
-  <si>
-    <t>anechoicspoof@gmail.com</t>
-  </si>
-  <si>
-    <t>mirado.rabenasolo@telecom-paris.fr</t>
-  </si>
-  <si>
-    <t>javier.velasquezgil@gmail.com</t>
-  </si>
-  <si>
-    <t>paul.olivier@eurecom.fr</t>
-  </si>
-  <si>
-    <t>1826273875@qq.com</t>
-  </si>
-  <si>
-    <t>2625936438@qq.com</t>
-  </si>
-  <si>
-    <t>teo.hays@protonmail.com</t>
-  </si>
-  <si>
-    <t>songrittom@gmail.com</t>
-  </si>
-  <si>
-    <t>ahmad.bazzi@ceva-dsp.com</t>
-  </si>
-  <si>
-    <t>nahel12789@gmail.com</t>
-  </si>
-  <si>
-    <t>abedifarv@gmail.com</t>
-  </si>
-  <si>
-    <t>mhd.nouri@yahoo.com</t>
-  </si>
-  <si>
-    <t>huy.ngo@eurecom.fr</t>
-  </si>
-  <si>
-    <t>ramon.fontes@imd.ufrn.br</t>
-  </si>
-  <si>
-    <t>aqadeer000@citymail.cuny.edu</t>
-  </si>
-  <si>
-    <t>arthur.bureau1@etu.univ-nantes.fr</t>
-  </si>
-  <si>
-    <t>pascal.tempier@inria.fr</t>
-  </si>
-  <si>
-    <t>ftester@ilabt.imec.be.stub</t>
-  </si>
-  <si>
-    <t>mohamed.lahsini@inria.fr</t>
-  </si>
-  <si>
-    <t>raza.ul-mustafa@inria.fr</t>
-  </si>
-  <si>
-    <t>theodoros.tsourdinis@lip6.fr</t>
-  </si>
-  <si>
-    <t>vinod.khandkar@inria.fr</t>
-  </si>
-  <si>
-    <t>yhadjadj@irisa.fr</t>
-  </si>
-  <si>
-    <t>anne-josiane.kouam-djuigne@inria.fr</t>
-  </si>
-  <si>
-    <t>noschmid@student.ethz.ch</t>
-  </si>
-  <si>
-    <t>mamoutou.diarra@hivenet.com</t>
-  </si>
-  <si>
-    <t>robbie.drage@spsautomation.com</t>
-  </si>
-  <si>
-    <t>sindi@innovatechtelecom.com</t>
-  </si>
-  <si>
-    <t>boutiba@eurecom.fr</t>
-  </si>
-  <si>
-    <t>g.pantaleo5@studenti.poliba.it</t>
-  </si>
-  <si>
-    <t>markrosenbaum@wearehackerone.com</t>
-  </si>
-  <si>
-    <t>jose.moura@iscte-iul.pt</t>
-  </si>
-  <si>
-    <t>sagar.arora@eurecom.fr</t>
-  </si>
-  <si>
-    <t>aya.moheddine@inria.fr</t>
-  </si>
-  <si>
-    <t>jiali.xu@inria.fr</t>
-  </si>
-  <si>
-    <t>selma.yahia@inria.fr</t>
-  </si>
-  <si>
-    <t>amamiyassir@gmail.com</t>
-  </si>
-  <si>
-    <t>rakesh.mundlamuri@eurecom.fr</t>
-  </si>
-  <si>
-    <t>nmkirimi@gmail.com</t>
-  </si>
-  <si>
-    <t>sanaa.ghandi@inria.fr</t>
-  </si>
-  <si>
-    <t>gitlab.runner@turletti.com</t>
-  </si>
-  <si>
-    <t>nbhatia3@ucsc.edu</t>
-  </si>
-  <si>
-    <t>saadtzl.2002@gmail.com</t>
-  </si>
-  <si>
-    <t>parsa.rajabzadeh@nokia.com</t>
-  </si>
-  <si>
-    <t>gallenmu@net.in.tum.de</t>
-  </si>
-  <si>
-    <t>fitowh@gmail.com</t>
-  </si>
-  <si>
-    <t>mattia.ciaccia@inria.fr</t>
-  </si>
-  <si>
-    <t>maros.plsik@tuvsud.com</t>
-  </si>
-  <si>
-    <t>mohammadbagher.tavassoli-kejani@inria.fr</t>
+    <t>After leaving Inria</t>
+  </si>
+  <si>
+    <t>PhD student in DIANA</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/jaroslaw-frelek-60306ab5/?originalSubdomain=pl</t>
+  </si>
+  <si>
+    <t>Pologne</t>
+  </si>
+  <si>
+    <t>https://wwsi.edu.pl/</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>https://github.com/lfarizav</t>
+  </si>
+  <si>
+    <t>Colombie</t>
+  </si>
+  <si>
+    <t>https://github.com/wborbaneto</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/assia-canina/?originalSubdomain=ca</t>
+  </si>
+  <si>
+    <t>A l'époque stagiaire chez nous (en plein covid)</t>
+  </si>
+  <si>
+    <t>https://scholar.google.es/citations?user=CIwBpVkAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=dASs7vgAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>https://www.vt.edu/</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Atanas-Vlahov</t>
+  </si>
+  <si>
+    <t>Bulgarie</t>
+  </si>
+  <si>
+    <t>OAI</t>
+  </si>
+  <si>
+    <t>Royaume Uni</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Leigh-Porter, https://www.roke.co.uk/</t>
+  </si>
+  <si>
+    <t>https://idtolu.com/</t>
+  </si>
+  <si>
+    <t>https://www.uajs.edu.co/</t>
+  </si>
+  <si>
+    <t>https://unisucre.edu.co/estructura-organica/, Martinez Francisco</t>
+  </si>
+  <si>
+    <t>Chine</t>
+  </si>
+  <si>
+    <t>Inconnu</t>
+  </si>
+  <si>
+    <t>A vérifier s'il a été validé et s'il a réservé ou pas</t>
+  </si>
+  <si>
+    <t>Apprenti chez DIANA</t>
+  </si>
+  <si>
+    <t>https://therealbazzi.github.io/</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>https://www.ku.ac.th/en/community-home, Kasetsart University, Thailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vahid Abedifar </t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Pascal</t>
+  </si>
+  <si>
+    <t>Stagiaire DIANA</t>
+  </si>
+  <si>
+    <t>SLICES et non plus FIT</t>
+  </si>
+  <si>
+    <t>Vinod, post-doc DIANA</t>
+  </si>
+  <si>
+    <t>Suisse</t>
+  </si>
+  <si>
+    <t>Mamoutou est parti chez HIVE</t>
+  </si>
+  <si>
+    <t>Nouvelle Zelande</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/rdrage/?originalSubdomain=nz</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/j-sindi-yamamoto-7679758/?originalSubdomain=br</t>
+  </si>
+  <si>
+    <t>Etudiant PoliBa stagiaire chez nous</t>
+  </si>
+  <si>
+    <t>hacker, voir https://cert.europa.eu/hall-of-fame</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>https://ciencia.iscte-iul.pt/authors/jose-moura/cv</t>
+  </si>
+  <si>
+    <t>TER chez nous</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/maros-plsik/?originalSubdomain=cz</t>
+  </si>
+  <si>
+    <t>République Techèque</t>
+  </si>
+  <si>
+    <t>Allemagne</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/parsa-rajabzadeh/</t>
+  </si>
+  <si>
+    <t>https://campusdirectory.ucsc.edu/cd_detail?uid=nbhatia3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1081,19 +1237,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF839496"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1117,7 +1273,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1136,7 +1292,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1485,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K220"/>
+  <dimension ref="A1:L220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="G212" sqref="G212"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="D158" sqref="D158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1496,8 +1655,8 @@
     <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
     <col min="2" max="3" width="7" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="51.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
     <col min="8" max="10" width="10.83203125" style="1"/>
   </cols>
@@ -5760,7 +5919,7 @@
       <c r="D133" s="1">
         <v>167</v>
       </c>
-      <c r="E133" s="5" t="s">
+      <c r="E133" t="s">
         <v>234</v>
       </c>
       <c r="F133" s="1" t="s">
@@ -5815,1207 +5974,2624 @@
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A135" s="8">
+      <c r="A135" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B135" s="1">
+        <v>4</v>
+      </c>
+      <c r="C135" s="1">
+        <v>10</v>
+      </c>
+      <c r="D135" s="1">
+        <v>169</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I135" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J135" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B136" s="1">
+        <v>4</v>
+      </c>
+      <c r="C136" s="1">
+        <v>18</v>
+      </c>
+      <c r="D136" s="1">
+        <v>170</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I136" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J136" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B137" s="1">
+        <v>4</v>
+      </c>
+      <c r="C137" s="1">
+        <v>19</v>
+      </c>
+      <c r="D137" s="1">
+        <v>171</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I137" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B138" s="1">
+        <v>4</v>
+      </c>
+      <c r="C138" s="1">
+        <v>22</v>
+      </c>
+      <c r="D138" s="1">
+        <v>172</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I138" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B139" s="1">
+        <v>5</v>
+      </c>
+      <c r="C139" s="1">
+        <v>2</v>
+      </c>
+      <c r="D139" s="1">
+        <v>173</v>
+      </c>
+      <c r="E139" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I139" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J139" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B140" s="1">
+        <v>5</v>
+      </c>
+      <c r="C140" s="1">
+        <v>21</v>
+      </c>
+      <c r="D140" s="1">
+        <v>174</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I140" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J140" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B141" s="1">
+        <v>7</v>
+      </c>
+      <c r="C141" s="1">
+        <v>9</v>
+      </c>
+      <c r="D141" s="1">
+        <v>175</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I141" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J141" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B142" s="1">
+        <v>10</v>
+      </c>
+      <c r="C142" s="1">
+        <v>7</v>
+      </c>
+      <c r="D142" s="1">
+        <v>176</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I142" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J142" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B143" s="1">
+        <v>10</v>
+      </c>
+      <c r="C143" s="1">
+        <v>24</v>
+      </c>
+      <c r="D143" s="1">
+        <v>177</v>
+      </c>
+      <c r="E143" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J143" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B144" s="1">
+        <v>11</v>
+      </c>
+      <c r="C144" s="1">
+        <v>5</v>
+      </c>
+      <c r="D144" s="1">
+        <v>178</v>
+      </c>
+      <c r="E144" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I144" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J144" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B145" s="1">
+        <v>11</v>
+      </c>
+      <c r="C145" s="1">
+        <v>14</v>
+      </c>
+      <c r="D145" s="1">
+        <v>179</v>
+      </c>
+      <c r="E145" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I145" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J145" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K145" s="6"/>
+      <c r="L145" s="6"/>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
         <v>2017</v>
       </c>
-      <c r="B135" s="8">
+      <c r="B146" s="1">
         <v>4</v>
       </c>
-      <c r="C135" s="8">
+      <c r="C146" s="1">
         <v>11</v>
       </c>
-      <c r="E135" s="8" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A136" s="8">
+      <c r="D146" s="1">
+        <v>180</v>
+      </c>
+      <c r="E146" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H146" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I146" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J146" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K146" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="L146" s="6"/>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
         <v>2019</v>
       </c>
-      <c r="B136" s="8">
+      <c r="B147" s="1">
+        <v>12</v>
+      </c>
+      <c r="C147" s="1">
+        <v>13</v>
+      </c>
+      <c r="E147" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H147" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I147" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J147" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K147" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="L147" s="6"/>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B148" s="1">
+        <v>12</v>
+      </c>
+      <c r="C148" s="1">
+        <v>15</v>
+      </c>
+      <c r="E148" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H148" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I148" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J148" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K148" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="L148" s="6"/>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B149" s="1">
+        <v>1</v>
+      </c>
+      <c r="C149" s="1">
+        <v>13</v>
+      </c>
+      <c r="E149" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I149" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J149" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K149" s="6"/>
+      <c r="L149" s="6"/>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B150" s="1">
+        <v>2</v>
+      </c>
+      <c r="C150" s="1">
+        <v>5</v>
+      </c>
+      <c r="E150" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I150" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K150" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="L150" s="6"/>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B151" s="1">
+        <v>2</v>
+      </c>
+      <c r="C151" s="1">
+        <v>18</v>
+      </c>
+      <c r="E151" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I151" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J151" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K151" s="6"/>
+      <c r="L151" s="6"/>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B152" s="1">
+        <v>2</v>
+      </c>
+      <c r="C152" s="1">
+        <v>22</v>
+      </c>
+      <c r="E152" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H152" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I152" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J152" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K152" s="6"/>
+      <c r="L152" s="6"/>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B153" s="1">
+        <v>2</v>
+      </c>
+      <c r="C153" s="1">
+        <v>25</v>
+      </c>
+      <c r="E153" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I153" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J153" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K153" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="L153" s="6"/>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B154" s="1">
+        <v>2</v>
+      </c>
+      <c r="C154" s="1">
+        <v>27</v>
+      </c>
+      <c r="E154" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I154" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J154" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K154" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="L154" s="6"/>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B155" s="1">
+        <v>2</v>
+      </c>
+      <c r="C155" s="1">
+        <v>28</v>
+      </c>
+      <c r="E155" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H155" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I155" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J155" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K155" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="L155" s="6"/>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B156" s="1">
+        <v>3</v>
+      </c>
+      <c r="C156" s="1">
+        <v>2</v>
+      </c>
+      <c r="E156" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H156" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I156" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J156" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K156" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="L156" s="6"/>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B157" s="1">
+        <v>3</v>
+      </c>
+      <c r="C157" s="1">
         <v>4</v>
       </c>
-      <c r="C136" s="8">
+      <c r="E157" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H157" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I157" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J157" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K157" s="6"/>
+      <c r="L157" s="6"/>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B158" s="1">
+        <v>3</v>
+      </c>
+      <c r="C158" s="1">
+        <v>5</v>
+      </c>
+      <c r="E158" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H158" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I158" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J158" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K158" s="6"/>
+      <c r="L158" s="6"/>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B159" s="1">
+        <v>3</v>
+      </c>
+      <c r="C159" s="1">
+        <v>20</v>
+      </c>
+      <c r="E159" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G159" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H159" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I159" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J159" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K159" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="L159" s="6"/>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B160" s="1">
+        <v>3</v>
+      </c>
+      <c r="C160" s="1">
+        <v>20</v>
+      </c>
+      <c r="E160" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G160" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H160" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I160" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J160" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K160" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="L160" s="6"/>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B161" s="1">
+        <v>4</v>
+      </c>
+      <c r="C161" s="1">
+        <v>2</v>
+      </c>
+      <c r="E161" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H161" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I161" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J161" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K161" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="L161" s="6"/>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B162" s="1">
+        <v>5</v>
+      </c>
+      <c r="C162" s="1">
+        <v>8</v>
+      </c>
+      <c r="E162" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I162" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J162" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K162" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="L162" s="6"/>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A163" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B163" s="1">
+        <v>6</v>
+      </c>
+      <c r="C163" s="1">
+        <v>2</v>
+      </c>
+      <c r="E163" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F163" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="K163" s="6"/>
+      <c r="L163" s="6"/>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A164" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B164" s="1">
+        <v>6</v>
+      </c>
+      <c r="C164" s="1">
+        <v>3</v>
+      </c>
+      <c r="E164" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H164" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I164" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J164" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K164" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="L164" s="6"/>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B165" s="1">
+        <v>6</v>
+      </c>
+      <c r="C165" s="1">
         <v>10</v>
       </c>
-      <c r="E136" s="8" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A137" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B137" s="8">
+      <c r="E165" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I165" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J165" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K165" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="L165" s="6"/>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A166" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B166" s="1">
+        <v>7</v>
+      </c>
+      <c r="C166" s="1">
+        <v>2</v>
+      </c>
+      <c r="E166" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I166" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J166" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K166" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="L166" s="6"/>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A167" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B167" s="1">
+        <v>8</v>
+      </c>
+      <c r="C167" s="1">
+        <v>31</v>
+      </c>
+      <c r="E167" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I167" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J167" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K167" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="L167" s="6"/>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A168" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B168" s="1">
+        <v>11</v>
+      </c>
+      <c r="C168" s="1">
+        <v>16</v>
+      </c>
+      <c r="E168" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I168" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J168" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K168" s="6"/>
+      <c r="L168" s="6"/>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A169" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B169" s="1">
+        <v>11</v>
+      </c>
+      <c r="C169" s="1">
+        <v>23</v>
+      </c>
+      <c r="E169" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I169" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J169" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K169" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="L169" s="6"/>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A170" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B170" s="1">
+        <v>11</v>
+      </c>
+      <c r="C170" s="1">
+        <v>27</v>
+      </c>
+      <c r="E170" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J170" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K170" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="L170" s="6"/>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B171" s="1">
+        <v>11</v>
+      </c>
+      <c r="C171" s="1">
+        <v>27</v>
+      </c>
+      <c r="E171" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I171" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J171" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K171" s="6"/>
+      <c r="L171" s="6"/>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A172" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B172" s="1">
+        <v>11</v>
+      </c>
+      <c r="C172" s="1">
+        <v>29</v>
+      </c>
+      <c r="E172" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="F172" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="K172" s="6"/>
+      <c r="L172" s="6"/>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A173" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B173" s="1">
+        <v>11</v>
+      </c>
+      <c r="C173" s="1">
+        <v>29</v>
+      </c>
+      <c r="E173" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I173" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J173" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K173" s="6"/>
+      <c r="L173" s="6"/>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A174" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B174" s="1">
+        <v>1</v>
+      </c>
+      <c r="C174" s="1">
+        <v>20</v>
+      </c>
+      <c r="E174" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="F174" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="K174" s="6"/>
+      <c r="L174" s="6"/>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A175" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B175" s="1">
+        <v>3</v>
+      </c>
+      <c r="C175" s="1">
+        <v>31</v>
+      </c>
+      <c r="E175" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H175" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I175" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J175" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K175" s="6"/>
+      <c r="L175" s="6"/>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A176" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B176" s="1">
         <v>4</v>
       </c>
-      <c r="C137" s="8">
-        <v>18</v>
-      </c>
-      <c r="E137" s="8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A138" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B138" s="8">
+      <c r="C176" s="1">
+        <v>12</v>
+      </c>
+      <c r="E176" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="F176" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="K176" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="L176" s="6"/>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A177" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B177" s="1">
         <v>4</v>
       </c>
-      <c r="C138" s="8">
+      <c r="C177" s="1">
+        <v>12</v>
+      </c>
+      <c r="E177" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="F177" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="K177" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="L177" s="6"/>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A178" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B178" s="1">
+        <v>5</v>
+      </c>
+      <c r="C178" s="1">
+        <v>4</v>
+      </c>
+      <c r="E178" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I178" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J178" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K178" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="L178" s="6"/>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A179" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B179" s="1">
+        <v>5</v>
+      </c>
+      <c r="C179" s="1">
+        <v>6</v>
+      </c>
+      <c r="E179" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I179" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J179" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K179" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="L179" s="6"/>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A180" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B180" s="1">
+        <v>5</v>
+      </c>
+      <c r="C180" s="1">
+        <v>25</v>
+      </c>
+      <c r="E180" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G180" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H180" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I180" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J180" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K180" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="L180" s="6"/>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A181" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B181" s="1">
+        <v>5</v>
+      </c>
+      <c r="C181" s="1">
+        <v>26</v>
+      </c>
+      <c r="E181" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="F181" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="K181" s="6"/>
+      <c r="L181" s="6"/>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B182" s="1">
+        <v>6</v>
+      </c>
+      <c r="C182" s="1">
+        <v>6</v>
+      </c>
+      <c r="E182" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="G182" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I182" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J182" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K182" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="L182" s="6"/>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B183" s="1">
+        <v>6</v>
+      </c>
+      <c r="C183" s="1">
         <v>19</v>
       </c>
-      <c r="E138" s="8" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A139" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B139" s="8">
+      <c r="E183" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="F183" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="K183" s="6"/>
+      <c r="L183" s="6"/>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B184" s="1">
+        <v>7</v>
+      </c>
+      <c r="C184" s="1">
+        <v>15</v>
+      </c>
+      <c r="E184" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G184" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H184" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I184" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J184" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K184" s="6"/>
+      <c r="L184" s="6"/>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A185" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B185" s="1">
+        <v>9</v>
+      </c>
+      <c r="C185" s="1">
+        <v>15</v>
+      </c>
+      <c r="E185" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H185" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I185" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J185" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K185" s="6"/>
+      <c r="L185" s="6"/>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A186" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B186" s="1">
+        <v>10</v>
+      </c>
+      <c r="C186" s="1">
+        <v>19</v>
+      </c>
+      <c r="E186" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H186" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I186" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J186" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K186" s="6"/>
+      <c r="L186" s="6"/>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A187" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B187" s="1">
+        <v>11</v>
+      </c>
+      <c r="C187" s="1">
+        <v>22</v>
+      </c>
+      <c r="E187" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="F187" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H187" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I187" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J187" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K187" s="6"/>
+      <c r="L187" s="6"/>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A188" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B188" s="1">
+        <v>11</v>
+      </c>
+      <c r="C188" s="1">
+        <v>24</v>
+      </c>
+      <c r="E188" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H188" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I188" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J188" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K188" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="L188" s="6"/>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A189" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B189" s="1">
+        <v>12</v>
+      </c>
+      <c r="C189" s="1">
+        <v>3</v>
+      </c>
+      <c r="E189" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H189" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I189" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J189" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K189" s="6"/>
+      <c r="L189" s="6"/>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A190" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B190" s="1">
+        <v>3</v>
+      </c>
+      <c r="C190" s="1">
+        <v>23</v>
+      </c>
+      <c r="E190" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H190" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I190" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J190" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K190" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="L190" s="6"/>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B191" s="1">
+        <v>6</v>
+      </c>
+      <c r="C191" s="1">
+        <v>29</v>
+      </c>
+      <c r="E191" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G191" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H191" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I191" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J191" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K191" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="L191" s="6"/>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A192" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B192" s="1">
+        <v>7</v>
+      </c>
+      <c r="C192" s="1">
+        <v>11</v>
+      </c>
+      <c r="E192" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H192" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I192" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J192" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K192" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="L192" s="6"/>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A193" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B193" s="1">
+        <v>7</v>
+      </c>
+      <c r="C193" s="1">
+        <v>21</v>
+      </c>
+      <c r="E193" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H193" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I193" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J193" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K193" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="L193" s="6"/>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A194" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B194" s="1">
+        <v>9</v>
+      </c>
+      <c r="C194" s="1">
+        <v>13</v>
+      </c>
+      <c r="E194" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H194" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I194" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J194" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K194" s="6"/>
+      <c r="L194" s="6"/>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A195" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B195" s="1">
+        <v>9</v>
+      </c>
+      <c r="C195" s="1">
+        <v>16</v>
+      </c>
+      <c r="E195" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H195" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I195" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J195" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K195" s="6"/>
+      <c r="L195" s="6"/>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A196" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B196" s="1">
+        <v>9</v>
+      </c>
+      <c r="C196" s="1">
+        <v>29</v>
+      </c>
+      <c r="E196" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="G196" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H196" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I196" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J196" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K196" s="6"/>
+      <c r="L196" s="6"/>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A197" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B197" s="1">
+        <v>12</v>
+      </c>
+      <c r="C197" s="1">
+        <v>12</v>
+      </c>
+      <c r="E197" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G197" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H197" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I197" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J197" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K197" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="L197" s="6"/>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A198" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B198" s="1">
+        <v>12</v>
+      </c>
+      <c r="C198" s="1">
+        <v>13</v>
+      </c>
+      <c r="E198" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="G198" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H198" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I198" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J198" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K198" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="L198" s="6"/>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A199" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B199" s="1">
+        <v>12</v>
+      </c>
+      <c r="C199" s="1">
+        <v>20</v>
+      </c>
+      <c r="E199" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G199" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H199" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I199" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J199" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K199" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="L199" s="6"/>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B200" s="1">
+        <v>1</v>
+      </c>
+      <c r="C200" s="1">
+        <v>11</v>
+      </c>
+      <c r="E200" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G200" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H200" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I200" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J200" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K200" s="6"/>
+      <c r="L200" s="6"/>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A201" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B201" s="1">
+        <v>1</v>
+      </c>
+      <c r="C201" s="1">
+        <v>11</v>
+      </c>
+      <c r="E201" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G201" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H201" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I201" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J201" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K201" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="L201" s="6"/>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A202" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B202" s="1">
+        <v>2</v>
+      </c>
+      <c r="C202" s="1">
         <v>4</v>
       </c>
-      <c r="C139" s="8">
+      <c r="E202" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="F202" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="K202" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="L202" s="6"/>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A203" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B203" s="1">
+        <v>3</v>
+      </c>
+      <c r="C203" s="1">
+        <v>31</v>
+      </c>
+      <c r="E203" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="G203" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H203" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I203" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J203" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K203" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="L203" s="6"/>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A204" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B204" s="1">
+        <v>4</v>
+      </c>
+      <c r="C204" s="1">
+        <v>28</v>
+      </c>
+      <c r="E204" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G204" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H204" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I204" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J204" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K204" s="6"/>
+      <c r="L204" s="6"/>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A205" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B205" s="1">
+        <v>9</v>
+      </c>
+      <c r="C205" s="1">
+        <v>12</v>
+      </c>
+      <c r="E205" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G205" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H205" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I205" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J205" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A206" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B206" s="1">
+        <v>9</v>
+      </c>
+      <c r="C206" s="1">
+        <v>12</v>
+      </c>
+      <c r="E206" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G206" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H206" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I206" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J206" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A207" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B207" s="1">
+        <v>10</v>
+      </c>
+      <c r="C207" s="1">
+        <v>11</v>
+      </c>
+      <c r="E207" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G207" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H207" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I207" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J207" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A208" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B208" s="1">
+        <v>10</v>
+      </c>
+      <c r="C208" s="1">
+        <v>25</v>
+      </c>
+      <c r="E208" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G208" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H208" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I208" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J208" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K208" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A209" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B209" s="1">
+        <v>10</v>
+      </c>
+      <c r="C209" s="1">
+        <v>26</v>
+      </c>
+      <c r="E209" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G209" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H209" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I209" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J209" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A210" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B210" s="1">
+        <v>11</v>
+      </c>
+      <c r="C210" s="1">
+        <v>21</v>
+      </c>
+      <c r="E210" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="F210" s="9" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A211" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B211" s="1">
+        <v>1</v>
+      </c>
+      <c r="C211" s="1">
+        <v>8</v>
+      </c>
+      <c r="E211" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G211" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H211" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I211" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J211" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A212" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B212" s="1">
+        <v>2</v>
+      </c>
+      <c r="C212" s="1">
+        <v>2</v>
+      </c>
+      <c r="E212" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G212" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H212" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I212" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J212" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A213" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B213" s="1">
+        <v>2</v>
+      </c>
+      <c r="C213" s="1">
+        <v>8</v>
+      </c>
+      <c r="E213" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G213" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H213" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I213" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J213" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K213" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A214" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B214" s="1">
+        <v>3</v>
+      </c>
+      <c r="C214" s="1">
+        <v>15</v>
+      </c>
+      <c r="E214" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G214" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H214" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I214" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J214" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K214" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A215" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B215" s="1">
+        <v>3</v>
+      </c>
+      <c r="C215" s="1">
+        <v>29</v>
+      </c>
+      <c r="E215" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G215" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H215" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I215" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J215" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K215" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A216" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B216" s="1">
+        <v>4</v>
+      </c>
+      <c r="C216" s="1">
+        <v>24</v>
+      </c>
+      <c r="E216" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="G216" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H216" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I216" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J216" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A217" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B217" s="1">
+        <v>5</v>
+      </c>
+      <c r="C217" s="1">
+        <v>14</v>
+      </c>
+      <c r="E217" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="F217" s="9" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A218" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B218" s="1">
+        <v>5</v>
+      </c>
+      <c r="C218" s="1">
+        <v>15</v>
+      </c>
+      <c r="E218" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G218" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H218" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I218" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J218" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A219" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B219" s="1">
+        <v>5</v>
+      </c>
+      <c r="C219" s="1">
         <v>22</v>
       </c>
-      <c r="E139" s="8" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A140" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B140" s="8">
-        <v>5</v>
-      </c>
-      <c r="C140" s="8">
-        <v>2</v>
-      </c>
-      <c r="E140" s="8" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A141" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B141" s="8">
-        <v>5</v>
-      </c>
-      <c r="C141" s="8">
-        <v>21</v>
-      </c>
-      <c r="E141" s="8" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A142" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B142" s="8">
-        <v>7</v>
-      </c>
-      <c r="C142" s="8">
-        <v>9</v>
-      </c>
-      <c r="E142" s="8" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A143" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B143" s="8">
-        <v>10</v>
-      </c>
-      <c r="C143" s="8">
-        <v>7</v>
-      </c>
-      <c r="E143" s="8" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A144" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B144" s="8">
-        <v>10</v>
-      </c>
-      <c r="C144" s="8">
-        <v>24</v>
-      </c>
-      <c r="E144" s="8" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A145" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B145" s="8">
-        <v>11</v>
-      </c>
-      <c r="C145" s="8">
-        <v>5</v>
-      </c>
-      <c r="E145" s="8" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B146" s="8">
-        <v>11</v>
-      </c>
-      <c r="C146" s="8">
-        <v>14</v>
-      </c>
-      <c r="E146" s="8" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B147" s="8">
-        <v>12</v>
-      </c>
-      <c r="C147" s="8">
-        <v>13</v>
-      </c>
-      <c r="E147" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A148" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B148" s="8">
-        <v>12</v>
-      </c>
-      <c r="C148" s="8">
-        <v>15</v>
-      </c>
-      <c r="E148" s="8" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A149" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B149" s="8">
-        <v>1</v>
-      </c>
-      <c r="C149" s="8">
-        <v>13</v>
-      </c>
-      <c r="E149" s="8" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A150" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B150" s="8">
-        <v>2</v>
-      </c>
-      <c r="C150" s="8">
-        <v>5</v>
-      </c>
-      <c r="E150" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A151" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B151" s="8">
-        <v>2</v>
-      </c>
-      <c r="C151" s="8">
-        <v>18</v>
-      </c>
-      <c r="E151" s="8" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B152" s="8">
-        <v>2</v>
-      </c>
-      <c r="C152" s="8">
-        <v>22</v>
-      </c>
-      <c r="E152" s="8" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B153" s="8">
-        <v>2</v>
-      </c>
-      <c r="C153" s="8">
-        <v>25</v>
-      </c>
-      <c r="E153" s="8" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A154" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B154" s="8">
-        <v>2</v>
-      </c>
-      <c r="C154" s="8">
-        <v>27</v>
-      </c>
-      <c r="E154" s="8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A155" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B155" s="8">
-        <v>2</v>
-      </c>
-      <c r="C155" s="8">
-        <v>28</v>
-      </c>
-      <c r="E155" s="8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A156" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B156" s="8">
-        <v>3</v>
-      </c>
-      <c r="C156" s="8">
-        <v>2</v>
-      </c>
-      <c r="E156" s="8" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A157" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B157" s="8">
-        <v>3</v>
-      </c>
-      <c r="C157" s="8">
-        <v>4</v>
-      </c>
-      <c r="E157" s="8" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A158" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B158" s="8">
-        <v>3</v>
-      </c>
-      <c r="C158" s="8">
-        <v>5</v>
-      </c>
-      <c r="E158" s="8" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A159" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B159" s="8">
-        <v>3</v>
-      </c>
-      <c r="C159" s="8">
+      <c r="E219" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="G219" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H219" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I219" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J219" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K219" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A220" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B220" s="1">
+        <v>6</v>
+      </c>
+      <c r="C220" s="1">
         <v>20</v>
       </c>
-      <c r="E159" s="8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A160" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B160" s="8">
-        <v>3</v>
-      </c>
-      <c r="C160" s="8">
-        <v>20</v>
-      </c>
-      <c r="E160" s="8" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A161" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B161" s="8">
-        <v>4</v>
-      </c>
-      <c r="C161" s="8">
-        <v>2</v>
-      </c>
-      <c r="E161" s="8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A162" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B162" s="8">
-        <v>5</v>
-      </c>
-      <c r="C162" s="8">
-        <v>8</v>
-      </c>
-      <c r="E162" s="8" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A163" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B163" s="8">
-        <v>6</v>
-      </c>
-      <c r="C163" s="8">
-        <v>2</v>
-      </c>
-      <c r="E163" s="8" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A164" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B164" s="8">
-        <v>6</v>
-      </c>
-      <c r="C164" s="8">
-        <v>3</v>
-      </c>
-      <c r="E164" s="8" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A165" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B165" s="8">
-        <v>6</v>
-      </c>
-      <c r="C165" s="8">
-        <v>10</v>
-      </c>
-      <c r="E165" s="8" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A166" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B166" s="8">
-        <v>7</v>
-      </c>
-      <c r="C166" s="8">
-        <v>2</v>
-      </c>
-      <c r="E166" s="8" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A167" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B167" s="8">
-        <v>8</v>
-      </c>
-      <c r="C167" s="8">
-        <v>31</v>
-      </c>
-      <c r="E167" s="8" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A168" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B168" s="8">
-        <v>11</v>
-      </c>
-      <c r="C168" s="8">
-        <v>16</v>
-      </c>
-      <c r="E168" s="8" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A169" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B169" s="8">
-        <v>11</v>
-      </c>
-      <c r="C169" s="8">
-        <v>23</v>
-      </c>
-      <c r="E169" s="8" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A170" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B170" s="8">
-        <v>11</v>
-      </c>
-      <c r="C170" s="8">
-        <v>27</v>
-      </c>
-      <c r="E170" s="8" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A171" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B171" s="8">
-        <v>11</v>
-      </c>
-      <c r="C171" s="8">
-        <v>27</v>
-      </c>
-      <c r="E171" s="8" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A172" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B172" s="8">
-        <v>11</v>
-      </c>
-      <c r="C172" s="8">
-        <v>29</v>
-      </c>
-      <c r="E172" s="8" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A173" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B173" s="8">
-        <v>11</v>
-      </c>
-      <c r="C173" s="8">
-        <v>29</v>
-      </c>
-      <c r="E173" s="8" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A174" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B174" s="8">
-        <v>1</v>
-      </c>
-      <c r="C174" s="8">
-        <v>20</v>
-      </c>
-      <c r="E174" s="8" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A175" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B175" s="8">
-        <v>3</v>
-      </c>
-      <c r="C175" s="8">
-        <v>31</v>
-      </c>
-      <c r="E175" s="8" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A176" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B176" s="8">
-        <v>4</v>
-      </c>
-      <c r="C176" s="8">
-        <v>12</v>
-      </c>
-      <c r="E176" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A177" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B177" s="8">
-        <v>4</v>
-      </c>
-      <c r="C177" s="8">
-        <v>12</v>
-      </c>
-      <c r="E177" s="8" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A178" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B178" s="8">
-        <v>5</v>
-      </c>
-      <c r="C178" s="8">
-        <v>4</v>
-      </c>
-      <c r="E178" s="8" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A179" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B179" s="8">
-        <v>5</v>
-      </c>
-      <c r="C179" s="8">
-        <v>6</v>
-      </c>
-      <c r="E179" s="8" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A180" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B180" s="8">
-        <v>5</v>
-      </c>
-      <c r="C180" s="8">
-        <v>25</v>
-      </c>
-      <c r="E180" s="8" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A181" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B181" s="8">
-        <v>5</v>
-      </c>
-      <c r="C181" s="8">
-        <v>26</v>
-      </c>
-      <c r="E181" s="8" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A182" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B182" s="8">
-        <v>6</v>
-      </c>
-      <c r="C182" s="8">
-        <v>6</v>
-      </c>
-      <c r="E182" s="8" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A183" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B183" s="8">
-        <v>6</v>
-      </c>
-      <c r="C183" s="8">
-        <v>19</v>
-      </c>
-      <c r="E183" s="8" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A184" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B184" s="8">
-        <v>7</v>
-      </c>
-      <c r="C184" s="8">
-        <v>15</v>
-      </c>
-      <c r="E184" s="8" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A185" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B185" s="8">
-        <v>9</v>
-      </c>
-      <c r="C185" s="8">
-        <v>15</v>
-      </c>
-      <c r="E185" s="8" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A186" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B186" s="8">
-        <v>10</v>
-      </c>
-      <c r="C186" s="8">
-        <v>19</v>
-      </c>
-      <c r="E186" s="8" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A187" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B187" s="8">
-        <v>11</v>
-      </c>
-      <c r="C187" s="8">
-        <v>22</v>
-      </c>
-      <c r="E187" s="8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A188" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B188" s="8">
-        <v>11</v>
-      </c>
-      <c r="C188" s="8">
-        <v>24</v>
-      </c>
-      <c r="E188" s="8" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A189" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B189" s="8">
-        <v>12</v>
-      </c>
-      <c r="C189" s="8">
-        <v>3</v>
-      </c>
-      <c r="E189" s="8" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A190" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B190" s="8">
-        <v>3</v>
-      </c>
-      <c r="C190" s="8">
-        <v>23</v>
-      </c>
-      <c r="E190" s="8" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A191" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B191" s="8">
-        <v>6</v>
-      </c>
-      <c r="C191" s="8">
-        <v>29</v>
-      </c>
-      <c r="E191" s="8" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A192" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B192" s="8">
-        <v>7</v>
-      </c>
-      <c r="C192" s="8">
-        <v>11</v>
-      </c>
-      <c r="E192" s="8" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A193" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B193" s="8">
-        <v>7</v>
-      </c>
-      <c r="C193" s="8">
-        <v>21</v>
-      </c>
-      <c r="E193" s="8" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A194" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B194" s="8">
-        <v>9</v>
-      </c>
-      <c r="C194" s="8">
-        <v>13</v>
-      </c>
-      <c r="E194" s="8" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A195" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B195" s="8">
-        <v>9</v>
-      </c>
-      <c r="C195" s="8">
-        <v>16</v>
-      </c>
-      <c r="E195" s="8" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A196" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B196" s="8">
-        <v>9</v>
-      </c>
-      <c r="C196" s="8">
-        <v>29</v>
-      </c>
-      <c r="E196" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A197" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B197" s="8">
-        <v>12</v>
-      </c>
-      <c r="C197" s="8">
-        <v>12</v>
-      </c>
-      <c r="E197" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A198" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B198" s="8">
-        <v>12</v>
-      </c>
-      <c r="C198" s="8">
-        <v>13</v>
-      </c>
-      <c r="E198" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A199" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B199" s="8">
-        <v>12</v>
-      </c>
-      <c r="C199" s="8">
-        <v>20</v>
-      </c>
-      <c r="E199" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A200" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B200" s="8">
-        <v>1</v>
-      </c>
-      <c r="C200" s="8">
-        <v>11</v>
-      </c>
-      <c r="E200" s="8" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A201" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B201" s="8">
-        <v>1</v>
-      </c>
-      <c r="C201" s="8">
-        <v>11</v>
-      </c>
-      <c r="E201" s="8" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A202" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B202" s="8">
-        <v>2</v>
-      </c>
-      <c r="C202" s="8">
-        <v>4</v>
-      </c>
-      <c r="E202" s="8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A203" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B203" s="8">
-        <v>3</v>
-      </c>
-      <c r="C203" s="8">
-        <v>31</v>
-      </c>
-      <c r="E203" s="8" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A204" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B204" s="8">
-        <v>4</v>
-      </c>
-      <c r="C204" s="8">
-        <v>28</v>
-      </c>
-      <c r="E204" s="8" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A205" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B205" s="8">
-        <v>9</v>
-      </c>
-      <c r="C205" s="8">
-        <v>12</v>
-      </c>
-      <c r="E205" s="8" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A206" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B206" s="8">
-        <v>9</v>
-      </c>
-      <c r="C206" s="8">
-        <v>12</v>
-      </c>
-      <c r="E206" s="8" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A207" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B207" s="8">
-        <v>10</v>
-      </c>
-      <c r="C207" s="8">
-        <v>11</v>
-      </c>
-      <c r="E207" s="8" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A208" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B208" s="8">
-        <v>10</v>
-      </c>
-      <c r="C208" s="8">
-        <v>25</v>
-      </c>
-      <c r="E208" s="8" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A209" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B209" s="8">
-        <v>10</v>
-      </c>
-      <c r="C209" s="8">
-        <v>26</v>
-      </c>
-      <c r="E209" s="8" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A210" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B210" s="8">
-        <v>11</v>
-      </c>
-      <c r="C210" s="8">
-        <v>21</v>
-      </c>
-      <c r="E210" s="8" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A211" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B211" s="8">
-        <v>1</v>
-      </c>
-      <c r="C211" s="8">
-        <v>8</v>
-      </c>
-      <c r="E211" s="8" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A212" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B212" s="8">
-        <v>2</v>
-      </c>
-      <c r="C212" s="8">
-        <v>2</v>
-      </c>
-      <c r="E212" s="8" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A213" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B213" s="8">
-        <v>2</v>
-      </c>
-      <c r="C213" s="8">
-        <v>8</v>
-      </c>
-      <c r="E213" s="8" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A214" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B214" s="8">
-        <v>3</v>
-      </c>
-      <c r="C214" s="8">
-        <v>15</v>
-      </c>
-      <c r="E214" s="8" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A215" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B215" s="8">
-        <v>3</v>
-      </c>
-      <c r="C215" s="8">
-        <v>29</v>
-      </c>
-      <c r="E215" s="8" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A216" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B216" s="8">
-        <v>4</v>
-      </c>
-      <c r="C216" s="8">
-        <v>24</v>
-      </c>
-      <c r="E216" s="8" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A217" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B217" s="8">
-        <v>5</v>
-      </c>
-      <c r="C217" s="8">
-        <v>14</v>
-      </c>
-      <c r="E217" s="8" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A218" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B218" s="8">
-        <v>5</v>
-      </c>
-      <c r="C218" s="8">
-        <v>15</v>
-      </c>
-      <c r="E218" s="8" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A219" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B219" s="8">
-        <v>5</v>
-      </c>
-      <c r="C219" s="8">
-        <v>22</v>
-      </c>
-      <c r="E219" s="8" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A220" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B220" s="8">
-        <v>6</v>
-      </c>
-      <c r="C220" s="8">
-        <v>20</v>
-      </c>
-      <c r="E220" s="8" t="s">
-        <v>333</v>
+      <c r="E220" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G220" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H220" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I220" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J220" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -7026,7 +8602,17 @@
     <hyperlink ref="E125" r:id="rId4" xr:uid="{E11FAB11-FA2B-1F43-BBD9-DCF008AC5CD1}"/>
     <hyperlink ref="E126" r:id="rId5" xr:uid="{3EB2F7EB-F790-664D-B837-D3E3FB0757B6}"/>
     <hyperlink ref="E134" r:id="rId6" xr:uid="{1BD56906-84F7-3B49-84AA-A11760B0D79E}"/>
-    <hyperlink ref="E133" r:id="rId7" xr:uid="{8B4200FD-E008-6A49-9EBC-A49BF9ED620B}"/>
+    <hyperlink ref="E135" r:id="rId7" xr:uid="{3411BBC7-32B3-EA45-AE69-0FABD406A651}"/>
+    <hyperlink ref="E136" r:id="rId8" xr:uid="{201DDFE3-5ECC-5F47-B969-5FC8966E11C9}"/>
+    <hyperlink ref="E137" r:id="rId9" xr:uid="{00AD707D-0D3B-E44C-9426-4C230B55597D}"/>
+    <hyperlink ref="E138" r:id="rId10" xr:uid="{1FB5C678-9B51-0146-83FB-67D733B8CE1F}"/>
+    <hyperlink ref="E139" r:id="rId11" xr:uid="{4BE6EDC3-8998-9A44-8124-87229DAC34A8}"/>
+    <hyperlink ref="E140" r:id="rId12" xr:uid="{F831CE3D-1D75-8E43-BAB3-A4B4B88A88B8}"/>
+    <hyperlink ref="E141" r:id="rId13" xr:uid="{ECFBDC50-314D-9A4A-BCFD-BBC39C266FF3}"/>
+    <hyperlink ref="E142" r:id="rId14" xr:uid="{562652E6-C43F-AE49-A22A-B03167DD7A39}"/>
+    <hyperlink ref="E143" r:id="rId15" xr:uid="{F8399B70-B55A-2843-AF99-C313BA47EE82}"/>
+    <hyperlink ref="E144" r:id="rId16" xr:uid="{27B28A51-5934-7C4F-A3A9-AE849DF8335A}"/>
+    <hyperlink ref="E145" r:id="rId17" xr:uid="{57D1270B-5780-CC48-9C28-4E55FB500D14}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>